<commit_message>
Format factor data Excel file
</commit_message>
<xml_diff>
--- a/Cleaned_Factor_data.xlsx
+++ b/Cleaned_Factor_data.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11214"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/d.larsen/Kandidat_kode/kandidat/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCDF94D-A502-7E4C-BB2E-0D8A63437FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -256,8 +262,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,10 +315,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -320,13 +332,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -364,7 +384,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -398,6 +418,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -432,9 +453,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -607,238 +629,241 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:75">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:75" ht="32" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AI1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AK1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AL1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AM1" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AN1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AO1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AP1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AQ1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AR1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AS1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AT1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="AU1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="AV1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AW1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AX1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AY1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="AZ1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BA1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BB1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BC1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BD1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BE1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BF1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BG1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BH1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BI1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BK1" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BL1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BM1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BN1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BO1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BP1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BR1" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="BS1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BT1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="BU1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="BV1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="BW1" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:75">
+    <row r="2" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -849,7 +874,7 @@
         <v>2.93</v>
       </c>
       <c r="D2">
-        <v>0.58</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="E2">
         <v>3.7</v>
@@ -879,7 +904,7 @@
         <v>4.07</v>
       </c>
       <c r="N2">
-        <v>-2.55</v>
+        <v>-2.5499999999999998</v>
       </c>
       <c r="O2">
         <v>-8.98</v>
@@ -927,7 +952,7 @@
         <v>5.29</v>
       </c>
       <c r="AD2">
-        <v>4.52</v>
+        <v>4.5199999999999996</v>
       </c>
       <c r="AE2">
         <v>-1.66</v>
@@ -984,10 +1009,10 @@
         <v>12.64</v>
       </c>
       <c r="AW2">
-        <v>-1.09</v>
+        <v>-1.0900000000000001</v>
       </c>
       <c r="AX2">
-        <v>8.130000000000001</v>
+        <v>8.1300000000000008</v>
       </c>
       <c r="AY2">
         <v>-1.37</v>
@@ -1005,10 +1030,10 @@
         <v>4.2</v>
       </c>
       <c r="BD2">
-        <v>2.45</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="BE2">
-        <v>-4.6</v>
+        <v>-4.5999999999999996</v>
       </c>
       <c r="BF2">
         <v>-4.97</v>
@@ -1017,10 +1042,10 @@
         <v>-4.37</v>
       </c>
       <c r="BH2">
-        <v>9.210000000000001</v>
+        <v>9.2100000000000009</v>
       </c>
       <c r="BI2">
-        <v>5.06</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="BJ2">
         <v>-1.56</v>
@@ -1065,7 +1090,7 @@
         <v>2.68</v>
       </c>
     </row>
-    <row r="3" spans="1:75">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>75</v>
       </c>
@@ -1100,7 +1125,7 @@
         <v>0.93</v>
       </c>
       <c r="L3">
-        <v>2.07</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="M3">
         <v>2.79</v>
@@ -1109,7 +1134,7 @@
         <v>0.36</v>
       </c>
       <c r="O3">
-        <v>0.28</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="P3">
         <v>-4.22</v>
@@ -1232,7 +1257,7 @@
         <v>-2.38</v>
       </c>
       <c r="BD3">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="BE3">
         <v>-0.59</v>
@@ -1262,10 +1287,10 @@
         <v>0.64</v>
       </c>
       <c r="BN3">
-        <v>2.45</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="BO3">
-        <v>-1.11</v>
+        <v>-1.1100000000000001</v>
       </c>
       <c r="BP3">
         <v>1.9</v>
@@ -1283,7 +1308,7 @@
         <v>-0.65</v>
       </c>
       <c r="BU3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="BV3">
         <v>-3.63</v>
@@ -1292,7 +1317,7 @@
         <v>-2.76</v>
       </c>
     </row>
-    <row r="4" spans="1:75">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>76</v>
       </c>
@@ -1327,7 +1352,7 @@
         <v>-0.5</v>
       </c>
       <c r="L4">
-        <v>-2.24</v>
+        <v>-2.2400000000000002</v>
       </c>
       <c r="M4">
         <v>0.41</v>
@@ -1345,7 +1370,7 @@
         <v>-3.82</v>
       </c>
       <c r="R4">
-        <v>-4.14</v>
+        <v>-4.1399999999999997</v>
       </c>
       <c r="S4">
         <v>1.74</v>
@@ -1369,7 +1394,7 @@
         <v>-1.77</v>
       </c>
       <c r="Z4">
-        <v>-0.29</v>
+        <v>-0.28999999999999998</v>
       </c>
       <c r="AA4">
         <v>5.73</v>
@@ -1408,7 +1433,7 @@
         <v>12.09</v>
       </c>
       <c r="AM4">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="AN4">
         <v>0.4</v>
@@ -1435,13 +1460,13 @@
         <v>2.44</v>
       </c>
       <c r="AV4">
-        <v>-1.15</v>
+        <v>-1.1499999999999999</v>
       </c>
       <c r="AW4">
         <v>2.58</v>
       </c>
       <c r="AX4">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="AY4">
         <v>3.36</v>
@@ -1450,7 +1475,7 @@
         <v>-6.14</v>
       </c>
       <c r="BA4">
-        <v>1.14</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="BB4">
         <v>-1.23</v>
@@ -1519,7 +1544,7 @@
         <v>4.25</v>
       </c>
     </row>
-    <row r="5" spans="1:75">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>77</v>
       </c>
@@ -1557,7 +1582,7 @@
         <v>0.12</v>
       </c>
       <c r="M5">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="N5">
         <v>0.13</v>
@@ -1662,7 +1687,7 @@
         <v>0.23</v>
       </c>
       <c r="AV5">
-        <v>0.29</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="AW5">
         <v>0.33</v>
@@ -1746,7 +1771,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="6" spans="1:75">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>78</v>
       </c>
@@ -1754,13 +1779,13 @@
         <v>-2.23</v>
       </c>
       <c r="C6">
-        <v>-1.16</v>
+        <v>-1.1599999999999999</v>
       </c>
       <c r="D6">
         <v>4.51</v>
       </c>
       <c r="E6">
-        <v>-4.39</v>
+        <v>-4.3899999999999997</v>
       </c>
       <c r="F6">
         <v>8.5</v>
@@ -1781,7 +1806,7 @@
         <v>-1.22</v>
       </c>
       <c r="L6">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="M6">
         <v>1.66</v>
@@ -1811,7 +1836,7 @@
         <v>0.04</v>
       </c>
       <c r="V6">
-        <v>4.86</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="W6">
         <v>0.66</v>
@@ -1826,7 +1851,7 @@
         <v>2.39</v>
       </c>
       <c r="AA6">
-        <v>-4.52</v>
+        <v>-4.5199999999999996</v>
       </c>
       <c r="AB6">
         <v>-1.66</v>
@@ -1964,7 +1989,7 @@
         <v>3</v>
       </c>
       <c r="BU6">
-        <v>-0.5600000000000001</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="BV6">
         <v>0.63</v>

</xml_diff>